<commit_message>
initialize RSA of low and mid level features
</commit_message>
<xml_diff>
--- a/ecos_summary_table.xlsx
+++ b/ecos_summary_table.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDB1919-799C-47C0-AB82-8872A820CBA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15EF75D-C4F2-478D-A2B1-88B8F45AF94F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Glossary" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="197">
   <si>
     <t>filename</t>
   </si>
@@ -612,6 +612,12 @@
   </si>
   <si>
     <t>1=animate;0=inanimate. It mostly refers to whether the object can move or not</t>
+  </si>
+  <si>
+    <t>natural</t>
+  </si>
+  <si>
+    <t>animate</t>
   </si>
 </sst>
 </file>
@@ -1012,7 +1018,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -2957,8 +2963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2980,10 +2986,10 @@
         <v>188</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1</v>
+        <v>195</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -4684,7 +4690,7 @@
         <v>187</v>
       </c>
       <c r="C67">
-        <f t="shared" ref="C67:C96" si="2">VALUE(LEFT(A67,1))</f>
+        <f t="shared" ref="C67:C95" si="2">VALUE(LEFT(A67,1))</f>
         <v>5</v>
       </c>
       <c r="D67" t="str">
@@ -4692,7 +4698,7 @@
         <v>savannah</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" ref="E67:E96" si="3">MID(A67,2,FIND(".",A67)-2)</f>
+        <f t="shared" ref="E67:E95" si="3">MID(A67,2,FIND(".",A67)-2)</f>
         <v>18</v>
       </c>
       <c r="F67">

</xml_diff>